<commit_message>
Added SQL query screenshots and description on y-axis in line chart.
</commit_message>
<xml_diff>
--- a/exploring_weather_trends/exploring_weather_trends.xlsx
+++ b/exploring_weather_trends/exploring_weather_trends.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\God\Education\udacity-data-analyst\Exploring Weather Trends\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\God\Education\data-analyst-udacity\exploring_weather_trends\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410C3F7A-0D84-4E13-B29B-D7CF9F481081}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62C0C14-5D4C-46AE-90E0-AAC02714C77E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{A4B21D51-963B-4ABB-806E-6A04AFB86EEE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4B21D51-963B-4ABB-806E-6A04AFB86EEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Compare" sheetId="4" r:id="rId1"/>
@@ -2450,7 +2450,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3777,7 +3776,13 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Temperature</a:t>
+                  <a:t> Temperature (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ºC)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -5300,7 +5305,17 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Temperature</a:t>
+                  <a:t> Temperature (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ºC</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -6795,7 +6810,13 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Temperature</a:t>
+                  <a:t> Temperature (</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>ºC)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -8960,8 +8981,8 @@
   </sheetPr>
   <dimension ref="A1:C182"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="O54" sqref="O54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13135,7 +13156,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD53FF1-6940-4594-B8FE-66ECD1228638}">
   <dimension ref="A1:C184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
+    <sheetView topLeftCell="A164" workbookViewId="0">
       <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
@@ -13235,7 +13256,7 @@
         <v>7.69</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C8:C53" si="0">AVERAGE(B4:B10)</f>
+        <f t="shared" ref="C10:C53" si="0">AVERAGE(B4:B10)</f>
         <v>7.5857142857142845</v>
       </c>
     </row>

</xml_diff>